<commit_message>
Clickup pass task update
</commit_message>
<xml_diff>
--- a/Agedcare.xlsx
+++ b/Agedcare.xlsx
@@ -381,11 +381,11 @@
   </sheetPr>
   <dimension ref="B1:N19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O21" activeCellId="0" sqref="O21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.15"/>
@@ -994,10 +994,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -1059,10 +1059,10 @@
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.65"/>

</xml_diff>

<commit_message>
Clickup task pass/fail updated Complated
</commit_message>
<xml_diff>
--- a/Agedcare.xlsx
+++ b/Agedcare.xlsx
@@ -385,7 +385,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.15"/>
@@ -994,10 +994,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -1062,7 +1062,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.65"/>

</xml_diff>

<commit_message>
Click up task 8 pass
</commit_message>
<xml_diff>
--- a/Agedcare.xlsx
+++ b/Agedcare.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Table Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="77">
   <si>
     <t xml:space="preserve">Transaction ID</t>
   </si>
@@ -99,19 +99,16 @@
     <t xml:space="preserve">Facility 3</t>
   </si>
   <si>
+    <t xml:space="preserve">54eb5c05-efe3-4feb-b599-314ecc93cfb9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(bromocriptine) bromocriptine 5 mg capsule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External facility</t>
+  </si>
+  <si>
     <t xml:space="preserve">Windsor Charles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54eb5c05-efe3-4feb-b599-314ecc93cfb9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(bromocriptine) bromocriptine 5 mg capsule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">External facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wilbur Smith</t>
   </si>
   <si>
     <t xml:space="preserve">2aa9cdef-0d43-444f-95eb-e4a4c77ca455</t>
@@ -381,11 +378,11 @@
   </sheetPr>
   <dimension ref="B1:N19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.15"/>
@@ -490,7 +487,7 @@
         <v>24</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="3" t="n">
@@ -513,19 +510,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="3" t="n">
@@ -548,19 +545,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="3" t="n">
@@ -583,19 +580,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="3" t="n">
@@ -618,19 +615,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="3" t="n">
@@ -653,19 +650,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="3" t="n">
@@ -688,10 +685,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
@@ -700,7 +697,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="3" t="n">
@@ -723,19 +720,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="3" t="n">
@@ -758,19 +755,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3" t="n">
@@ -793,10 +790,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>15</v>
@@ -805,7 +802,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="3" t="n">
@@ -828,19 +825,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="3" t="n">
@@ -863,19 +860,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="3" t="n">
@@ -898,19 +895,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="3" t="n">
@@ -933,19 +930,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="3" t="n">
@@ -993,11 +990,11 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -1008,24 +1005,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>20</v>
@@ -1059,10 +1056,10 @@
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.65"/>
@@ -1071,15 +1068,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>1111</v>

</xml_diff>